<commit_message>
Finish Backend and FrontEnd
</commit_message>
<xml_diff>
--- a/backend/sorties.xlsx
+++ b/backend/sorties.xlsx
@@ -412,7 +412,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-04-28</v>
+        <v>2025-05-01</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -420,7 +420,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-04-29</v>
+        <v>2025-05-02</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -428,7 +428,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-04-30</v>
+        <v>2025-05-03</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -436,7 +436,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2025-05-01</v>
+        <v>2025-05-04</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -444,15 +444,15 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2025-05-02</v>
+        <v>2025-05-05</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2025-05-03</v>
+        <v>2025-05-06</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -460,18 +460,18 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2025-05-04</v>
+        <v>2025-05-07</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2025-05-05</v>
+        <v>2025-05-08</v>
       </c>
       <c r="B9">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>